<commit_message>
implement reading namedRegion from specific sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/namedRegions3.xlsx
+++ b/inst/extdata/namedRegions3.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="MyRange" vbProcedure="false">Sheet2!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">S1A1</t>
   </si>
@@ -36,7 +37,13 @@
     <t xml:space="preserve">S2A1</t>
   </si>
   <si>
-    <t xml:space="preserve">S2B2</t>
+    <t xml:space="preserve">S2A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S3A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S3B1</t>
   </si>
 </sst>
 </file>
@@ -139,11 +146,11 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -194,4 +201,36 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
unittests * improve test (use sheet name as well as sheet index) * Warning if wrong sheet was selected and no data * Warning if wrong namedRegion was selected
</commit_message>
<xml_diff>
--- a/inst/extdata/namedRegions3.xlsx
+++ b/inst/extdata/namedRegions3.xlsx
@@ -5,16 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet0" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" name="HiddenRange" vbProcedure="false">Sheet6!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" name="MyRange" vbProcedure="false">Sheet2!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="MyRange" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="MyRange" vbProcedure="false">Sheet3!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +31,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">S0A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S0B1</t>
+  </si>
   <si>
     <t xml:space="preserve">S1A1</t>
   </si>
@@ -37,13 +48,25 @@
     <t xml:space="preserve">S2A1</t>
   </si>
   <si>
-    <t xml:space="preserve">S2A2</t>
+    <t xml:space="preserve">S2B1</t>
   </si>
   <si>
     <t xml:space="preserve">S3A1</t>
   </si>
   <si>
     <t xml:space="preserve">S3B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S6B1</t>
   </si>
 </sst>
 </file>
@@ -53,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -74,6 +97,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="HiddenRange"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,12 +147,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,6 +179,134 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -154,24 +315,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -185,43 +346,11 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>